<commit_message>
Agrega puntuación a quiz
</commit_message>
<xml_diff>
--- a/public/docs/Holandés.xlsx
+++ b/public/docs/Holandés.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Optiva\Desktop\Web Development\Proyectos\sergio27.com\Holandés\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49827AE-592C-40A8-A24C-A280B8FC68C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50575873-8B00-43E2-95CA-2B0D2E8D3225}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C7366B0A-BB88-4025-AE92-B2E637926941}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Words" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="338">
   <si>
     <t>category</t>
   </si>
@@ -619,6 +619,435 @@
   </si>
   <si>
     <t>cuidar</t>
+  </si>
+  <si>
+    <t>Kleuren</t>
+  </si>
+  <si>
+    <t>rood</t>
+  </si>
+  <si>
+    <t>rojo</t>
+  </si>
+  <si>
+    <t>oranje</t>
+  </si>
+  <si>
+    <t>naranja</t>
+  </si>
+  <si>
+    <t>geel</t>
+  </si>
+  <si>
+    <t>amarillo</t>
+  </si>
+  <si>
+    <t>groen</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>blauw</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>paars</t>
+  </si>
+  <si>
+    <t>roze</t>
+  </si>
+  <si>
+    <t>rosa</t>
+  </si>
+  <si>
+    <t>morado</t>
+  </si>
+  <si>
+    <t>bruin</t>
+  </si>
+  <si>
+    <t>café</t>
+  </si>
+  <si>
+    <t>zwart</t>
+  </si>
+  <si>
+    <t>negro</t>
+  </si>
+  <si>
+    <t>wit</t>
+  </si>
+  <si>
+    <t>blanco</t>
+  </si>
+  <si>
+    <t>grijs</t>
+  </si>
+  <si>
+    <t>gris</t>
+  </si>
+  <si>
+    <t>mono</t>
+  </si>
+  <si>
+    <t>aap</t>
+  </si>
+  <si>
+    <t>oso</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>olifant</t>
+  </si>
+  <si>
+    <t>kangoeroe</t>
+  </si>
+  <si>
+    <t>giraffe</t>
+  </si>
+  <si>
+    <t>neushoorn</t>
+  </si>
+  <si>
+    <t>nijlpaard</t>
+  </si>
+  <si>
+    <t>leeuw</t>
+  </si>
+  <si>
+    <t>tijger</t>
+  </si>
+  <si>
+    <t>kameel</t>
+  </si>
+  <si>
+    <t>hert</t>
+  </si>
+  <si>
+    <t>slang</t>
+  </si>
+  <si>
+    <t>krokodil</t>
+  </si>
+  <si>
+    <t>schildpad</t>
+  </si>
+  <si>
+    <t>hagedis</t>
+  </si>
+  <si>
+    <t>salamander</t>
+  </si>
+  <si>
+    <t>kikker</t>
+  </si>
+  <si>
+    <t>pad</t>
+  </si>
+  <si>
+    <t>eend</t>
+  </si>
+  <si>
+    <t>zwaan</t>
+  </si>
+  <si>
+    <t>gans</t>
+  </si>
+  <si>
+    <t>mus</t>
+  </si>
+  <si>
+    <t>duif</t>
+  </si>
+  <si>
+    <t>merel</t>
+  </si>
+  <si>
+    <t>meeuw</t>
+  </si>
+  <si>
+    <t>roofvogel</t>
+  </si>
+  <si>
+    <t>uil</t>
+  </si>
+  <si>
+    <t>struisvogel</t>
+  </si>
+  <si>
+    <t>pinguin</t>
+  </si>
+  <si>
+    <t>papegaai</t>
+  </si>
+  <si>
+    <t>zeehond</t>
+  </si>
+  <si>
+    <t>dolfijn</t>
+  </si>
+  <si>
+    <t>haai</t>
+  </si>
+  <si>
+    <t>vis</t>
+  </si>
+  <si>
+    <t>orka</t>
+  </si>
+  <si>
+    <t>spin</t>
+  </si>
+  <si>
+    <t>bij</t>
+  </si>
+  <si>
+    <t>wesp</t>
+  </si>
+  <si>
+    <t>mug</t>
+  </si>
+  <si>
+    <t>vlieg</t>
+  </si>
+  <si>
+    <t>mier</t>
+  </si>
+  <si>
+    <t>rups</t>
+  </si>
+  <si>
+    <t>vliender</t>
+  </si>
+  <si>
+    <t>kever</t>
+  </si>
+  <si>
+    <t>hond</t>
+  </si>
+  <si>
+    <t>kat</t>
+  </si>
+  <si>
+    <t>konijn</t>
+  </si>
+  <si>
+    <t>cavia</t>
+  </si>
+  <si>
+    <t>muis</t>
+  </si>
+  <si>
+    <t>rat</t>
+  </si>
+  <si>
+    <t>hamster</t>
+  </si>
+  <si>
+    <t>goudvis</t>
+  </si>
+  <si>
+    <t>koe</t>
+  </si>
+  <si>
+    <t>stier</t>
+  </si>
+  <si>
+    <t>paard</t>
+  </si>
+  <si>
+    <t>varken</t>
+  </si>
+  <si>
+    <t>ezel</t>
+  </si>
+  <si>
+    <t>schaap</t>
+  </si>
+  <si>
+    <t>kip</t>
+  </si>
+  <si>
+    <t>haan</t>
+  </si>
+  <si>
+    <t>elefante</t>
+  </si>
+  <si>
+    <t>canguro</t>
+  </si>
+  <si>
+    <t>jirafa</t>
+  </si>
+  <si>
+    <t>rinoceronte</t>
+  </si>
+  <si>
+    <t>hipopótamo</t>
+  </si>
+  <si>
+    <t>león</t>
+  </si>
+  <si>
+    <t>tigre</t>
+  </si>
+  <si>
+    <t>camello</t>
+  </si>
+  <si>
+    <t>venado</t>
+  </si>
+  <si>
+    <t>serpiente</t>
+  </si>
+  <si>
+    <t>cocodrilo</t>
+  </si>
+  <si>
+    <t>tortuga</t>
+  </si>
+  <si>
+    <t>lagargo</t>
+  </si>
+  <si>
+    <t>salamandra</t>
+  </si>
+  <si>
+    <t>rana</t>
+  </si>
+  <si>
+    <t>sapo</t>
+  </si>
+  <si>
+    <t>pato</t>
+  </si>
+  <si>
+    <t>cisne</t>
+  </si>
+  <si>
+    <t>ganso</t>
+  </si>
+  <si>
+    <t>gorrión</t>
+  </si>
+  <si>
+    <t>paloma</t>
+  </si>
+  <si>
+    <t>mirlo</t>
+  </si>
+  <si>
+    <t>gaviota</t>
+  </si>
+  <si>
+    <t>ave de presa</t>
+  </si>
+  <si>
+    <t>búho</t>
+  </si>
+  <si>
+    <t>avestruz</t>
+  </si>
+  <si>
+    <t>pingüino</t>
+  </si>
+  <si>
+    <t>loro</t>
+  </si>
+  <si>
+    <t>foca</t>
+  </si>
+  <si>
+    <t>delfín</t>
+  </si>
+  <si>
+    <t>tiburón</t>
+  </si>
+  <si>
+    <t>pez</t>
+  </si>
+  <si>
+    <t>orca</t>
+  </si>
+  <si>
+    <t>araña</t>
+  </si>
+  <si>
+    <t>abeja</t>
+  </si>
+  <si>
+    <t>avispa</t>
+  </si>
+  <si>
+    <t>mosquito</t>
+  </si>
+  <si>
+    <t>mosca</t>
+  </si>
+  <si>
+    <t>hormiga</t>
+  </si>
+  <si>
+    <t>oruga</t>
+  </si>
+  <si>
+    <t>mariposa</t>
+  </si>
+  <si>
+    <t>escarabajo</t>
+  </si>
+  <si>
+    <t>perro</t>
+  </si>
+  <si>
+    <t>gato</t>
+  </si>
+  <si>
+    <t>conejo</t>
+  </si>
+  <si>
+    <t>conejillo de indias</t>
+  </si>
+  <si>
+    <t>ratón</t>
+  </si>
+  <si>
+    <t>rata</t>
+  </si>
+  <si>
+    <t>pez dorado</t>
+  </si>
+  <si>
+    <t>vaca</t>
+  </si>
+  <si>
+    <t>toro</t>
+  </si>
+  <si>
+    <t>caballo</t>
+  </si>
+  <si>
+    <t>cerdo</t>
+  </si>
+  <si>
+    <t>burro</t>
+  </si>
+  <si>
+    <t>oveja</t>
+  </si>
+  <si>
+    <t>pollo</t>
+  </si>
+  <si>
+    <t>gallo</t>
+  </si>
+  <si>
+    <t>Dieren</t>
   </si>
 </sst>
 </file>
@@ -970,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F2F90F-D41C-4F02-8E9E-C874BA19457C}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113:B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,6 +2824,1000 @@
         <v>42</v>
       </c>
     </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>195</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>196</v>
+      </c>
+      <c r="D102" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>195</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>198</v>
+      </c>
+      <c r="D103" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>195</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>200</v>
+      </c>
+      <c r="D104" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>195</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>202</v>
+      </c>
+      <c r="D105" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>195</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>204</v>
+      </c>
+      <c r="D106" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>195</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>206</v>
+      </c>
+      <c r="D107" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>195</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108" t="s">
+        <v>207</v>
+      </c>
+      <c r="D108" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>195</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>210</v>
+      </c>
+      <c r="D109" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>195</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>212</v>
+      </c>
+      <c r="D110" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>195</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>214</v>
+      </c>
+      <c r="D111" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>195</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>216</v>
+      </c>
+      <c r="D112" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>337</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>219</v>
+      </c>
+      <c r="D113" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>337</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s">
+        <v>221</v>
+      </c>
+      <c r="D114" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>337</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115" t="s">
+        <v>222</v>
+      </c>
+      <c r="D115" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>337</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+      <c r="C116" t="s">
+        <v>223</v>
+      </c>
+      <c r="D116" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>337</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>224</v>
+      </c>
+      <c r="D117" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>337</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>225</v>
+      </c>
+      <c r="D118" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>337</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
+        <v>226</v>
+      </c>
+      <c r="D119" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>337</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120" t="s">
+        <v>227</v>
+      </c>
+      <c r="D120" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>337</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="C121" t="s">
+        <v>228</v>
+      </c>
+      <c r="D121" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>337</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>229</v>
+      </c>
+      <c r="D122" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>337</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>230</v>
+      </c>
+      <c r="D123" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>337</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>231</v>
+      </c>
+      <c r="D124" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>337</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s">
+        <v>232</v>
+      </c>
+      <c r="D125" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>337</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>233</v>
+      </c>
+      <c r="D126" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>337</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>234</v>
+      </c>
+      <c r="D127" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>337</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>235</v>
+      </c>
+      <c r="D128" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>337</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>236</v>
+      </c>
+      <c r="D129" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>337</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>237</v>
+      </c>
+      <c r="D130" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>337</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="C131" t="s">
+        <v>238</v>
+      </c>
+      <c r="D131" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>337</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132" t="s">
+        <v>239</v>
+      </c>
+      <c r="D132" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>337</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>240</v>
+      </c>
+      <c r="D133" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>337</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>241</v>
+      </c>
+      <c r="D134" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>337</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+      <c r="C135" t="s">
+        <v>242</v>
+      </c>
+      <c r="D135" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>337</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>243</v>
+      </c>
+      <c r="D136" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>337</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>244</v>
+      </c>
+      <c r="D137" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>337</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138" t="s">
+        <v>245</v>
+      </c>
+      <c r="D138" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>337</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s">
+        <v>246</v>
+      </c>
+      <c r="D139" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>337</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
+        <v>247</v>
+      </c>
+      <c r="D140" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>337</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>248</v>
+      </c>
+      <c r="D141" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>337</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
+        <v>249</v>
+      </c>
+      <c r="D142" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>337</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
+        <v>250</v>
+      </c>
+      <c r="D143" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>337</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
+        <v>251</v>
+      </c>
+      <c r="D144" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>337</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145" t="s">
+        <v>252</v>
+      </c>
+      <c r="D145" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>337</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s">
+        <v>253</v>
+      </c>
+      <c r="D146" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>337</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+      <c r="C147" t="s">
+        <v>254</v>
+      </c>
+      <c r="D147" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>337</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+      <c r="C148" t="s">
+        <v>255</v>
+      </c>
+      <c r="D148" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>337</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="C149" t="s">
+        <v>256</v>
+      </c>
+      <c r="D149" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>337</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+      <c r="C150" t="s">
+        <v>257</v>
+      </c>
+      <c r="D150" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>337</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s">
+        <v>258</v>
+      </c>
+      <c r="D151" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>337</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>259</v>
+      </c>
+      <c r="D152" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>337</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="C153" t="s">
+        <v>260</v>
+      </c>
+      <c r="D153" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>337</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+      <c r="C154" t="s">
+        <v>261</v>
+      </c>
+      <c r="D154" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>337</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>262</v>
+      </c>
+      <c r="D155" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>337</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="C156" t="s">
+        <v>263</v>
+      </c>
+      <c r="D156" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>337</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="C157" t="s">
+        <v>264</v>
+      </c>
+      <c r="D157" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>337</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+      <c r="C158" t="s">
+        <v>265</v>
+      </c>
+      <c r="D158" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>337</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="C159" t="s">
+        <v>266</v>
+      </c>
+      <c r="D159" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>337</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>267</v>
+      </c>
+      <c r="D160" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>337</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="C161" t="s">
+        <v>268</v>
+      </c>
+      <c r="D161" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>337</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="C162" t="s">
+        <v>269</v>
+      </c>
+      <c r="D162" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>337</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163" t="s">
+        <v>270</v>
+      </c>
+      <c r="D163" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>337</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164" t="s">
+        <v>271</v>
+      </c>
+      <c r="D164" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>337</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165" t="s">
+        <v>272</v>
+      </c>
+      <c r="D165" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>337</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="C166" t="s">
+        <v>273</v>
+      </c>
+      <c r="D166" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>337</v>
+      </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
+      <c r="C167" t="s">
+        <v>274</v>
+      </c>
+      <c r="D167" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>337</v>
+      </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
+        <v>275</v>
+      </c>
+      <c r="D168" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>337</v>
+      </c>
+      <c r="B169">
+        <v>1</v>
+      </c>
+      <c r="C169" t="s">
+        <v>276</v>
+      </c>
+      <c r="D169" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>337</v>
+      </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
+      <c r="C170" t="s">
+        <v>277</v>
+      </c>
+      <c r="D170" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>337</v>
+      </c>
+      <c r="B171">
+        <v>1</v>
+      </c>
+      <c r="C171" t="s">
+        <v>278</v>
+      </c>
+      <c r="D171" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>337</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+      <c r="C172" t="s">
+        <v>279</v>
+      </c>
+      <c r="D172" t="s">
+        <v>336</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D102">
     <sortCondition ref="B67:B102"/>

</xml_diff>